<commit_message>
generate count_sheet with formatting on proper spots
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="MaddenCo Data {Date}" sheetId="1" r:id="rId1"/>
+    <sheet name="MaddenCo Counts {Date}" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="76">
   <si>
     <t>Date Created</t>
   </si>
@@ -230,13 +231,25 @@
   </si>
   <si>
     <t>16:58:41</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Immed</t>
+  </si>
+  <si>
+    <t>Later</t>
+  </si>
+  <si>
+    <t>Emails</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,6 +262,14 @@
       <color theme="1"/>
       <name val="Calibri Light"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -310,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -323,6 +344,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2030,4 +2054,144 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" s="5">
+        <v>142</v>
+      </c>
+      <c r="C1" s="5">
+        <v>154</v>
+      </c>
+      <c r="D1" s="5">
+        <v>161</v>
+      </c>
+      <c r="E1" s="5">
+        <v>124</v>
+      </c>
+      <c r="F1" s="5">
+        <v>138</v>
+      </c>
+      <c r="G1" s="5">
+        <v>149</v>
+      </c>
+      <c r="H1" s="5">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>14</v>
+      </c>
+      <c r="F2">
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
converted plain functions into an iterative OOP approach
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -339,14 +339,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -663,25 +663,25 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
@@ -2063,131 +2063,144 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="B1" s="5">
-        <v>142</v>
-      </c>
-      <c r="C1" s="5">
-        <v>154</v>
-      </c>
-      <c r="D1" s="5">
-        <v>161</v>
-      </c>
-      <c r="E1" s="5">
-        <v>124</v>
-      </c>
-      <c r="F1" s="5">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="4">
         <v>138</v>
       </c>
       <c r="G1" s="5">
         <v>149</v>
       </c>
-      <c r="H1" s="5">
+      <c r="H1" s="4">
         <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>7</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>5</v>
       </c>
-      <c r="E2">
-        <v>14</v>
-      </c>
-      <c r="F2">
+      <c r="E2" s="1">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1">
         <v>12</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>1</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>3</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>3</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>4</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>8</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>4</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>2</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>10</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>4</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>1</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>4</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>3</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>3</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>2</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>1</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="1">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
successfully generated a formatted Excel file from class approach
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="MaddenCo Data {Date}" sheetId="1" r:id="rId1"/>
-    <sheet name="MaddenCo Counts {Date}" sheetId="2" r:id="rId2"/>
+    <sheet name="MaddenCo Data 09-02-2022" sheetId="1" r:id="rId1"/>
+    <sheet name="MaddenCo Count 09-02-2022" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -339,14 +339,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -663,25 +663,25 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
@@ -2064,59 +2064,55 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1" max="2" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2" max="3" width="25.7109375" style="2" customWidth="1"/>
+    <col min="3" max="4" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="25.7109375" style="2" customWidth="1"/>
+    <col min="5" max="6" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6" max="7" width="25.7109375" style="2" customWidth="1"/>
+    <col min="7" max="8" width="25.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3">
+        <v>142</v>
+      </c>
+      <c r="C1" s="4">
+        <v>154</v>
+      </c>
+      <c r="D1" s="3">
+        <v>161</v>
+      </c>
+      <c r="E1" s="4">
+        <v>124</v>
+      </c>
+      <c r="F1" s="3">
+        <v>138</v>
+      </c>
+      <c r="G1" s="4">
+        <v>149</v>
+      </c>
+      <c r="H1" s="3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" s="4">
-        <v>138</v>
-      </c>
-      <c r="G1" s="5">
-        <v>149</v>
-      </c>
-      <c r="H1" s="4">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>5</v>
       </c>
       <c r="C2" s="1">
         <v>7</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>5</v>
       </c>
       <c r="E2" s="1">
         <v>14</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="2">
         <v>12</v>
       </c>
       <c r="G2" s="1">
@@ -2127,22 +2123,22 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>2</v>
       </c>
       <c r="C3" s="1">
         <v>3</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>3</v>
       </c>
       <c r="E3" s="1">
         <v>4</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="2">
         <v>8</v>
       </c>
       <c r="G3" s="1">
@@ -2153,22 +2149,22 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>3</v>
       </c>
       <c r="C4" s="1">
         <v>4</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>2</v>
       </c>
       <c r="E4" s="1">
         <v>10</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="2">
         <v>4</v>
       </c>
       <c r="G4" s="1">
@@ -2179,22 +2175,22 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>3</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>3</v>
       </c>
       <c r="E5" s="1">
         <v>3</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="2">
         <v>2</v>
       </c>
       <c r="G5" s="1">

</xml_diff>

<commit_message>
fixed bug with alternative column formatting with buffer
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="MaddenCo Data 09-02-2022" sheetId="1" r:id="rId1"/>
-    <sheet name="MaddenCo Count 09-02-2022" sheetId="2" r:id="rId2"/>
+    <sheet name="MaddenCo Data 02-09-2022" sheetId="1" r:id="rId1"/>
+    <sheet name="MaddenCo Count 02-09-2022" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -272,7 +272,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -300,6 +300,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDAEEF3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDE9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF79646"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4BACC6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -331,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -343,6 +367,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2064,139 +2100,140 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2" max="3" width="25.7109375" style="2" customWidth="1"/>
-    <col min="3" max="4" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="25.7109375" style="2" customWidth="1"/>
-    <col min="5" max="6" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6" max="7" width="25.7109375" style="2" customWidth="1"/>
-    <col min="7" max="8" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="B1" s="3">
+      <c r="B1" s="7">
         <v>142</v>
       </c>
-      <c r="C1" s="4">
+      <c r="C1" s="8">
         <v>154</v>
       </c>
-      <c r="D1" s="3">
+      <c r="D1" s="7">
         <v>161</v>
       </c>
-      <c r="E1" s="4">
+      <c r="E1" s="8">
         <v>124</v>
       </c>
-      <c r="F1" s="3">
+      <c r="F1" s="7">
         <v>138</v>
       </c>
-      <c r="G1" s="4">
+      <c r="G1" s="8">
         <v>149</v>
       </c>
-      <c r="H1" s="3">
+      <c r="H1" s="7">
         <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="6">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="5">
         <v>7</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="6">
         <v>5</v>
       </c>
-      <c r="E2" s="1">
-        <v>14</v>
-      </c>
-      <c r="F2" s="2">
+      <c r="E2" s="5">
+        <v>14</v>
+      </c>
+      <c r="F2" s="6">
         <v>12</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="5">
         <v>1</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="6">
         <v>2</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="5">
         <v>3</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="6">
         <v>3</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="5">
         <v>4</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="6">
         <v>8</v>
       </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1">
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="6">
         <v>3</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="5">
         <v>4</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="6">
         <v>2</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="5">
         <v>10</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="6">
         <v>4</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="5">
         <v>1</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="6">
         <v>3</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="5">
         <v>4</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="6">
         <v>3</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="5">
         <v>3</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="6">
         <v>2</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="5">
         <v>1</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="6">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added in row index formatting and file cleanup
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="76">
   <si>
     <t>Date Created</t>
   </si>
@@ -249,7 +249,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,14 +262,6 @@
       <color theme="1"/>
       <name val="Calibri Light"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -355,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -380,9 +372,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2134,7 +2123,7 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>72</v>
       </c>
       <c r="B2" s="6">
@@ -2160,7 +2149,7 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>73</v>
       </c>
       <c r="B3" s="6">
@@ -2186,7 +2175,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>74</v>
       </c>
       <c r="B4" s="6">
@@ -2212,7 +2201,7 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>75</v>
       </c>
       <c r="B5" s="6">

</xml_diff>

<commit_message>
bye bye AZ pt 2
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="MaddenCo Data 02-09-2022" sheetId="1" r:id="rId1"/>
-    <sheet name="MaddenCo Count 02-09-2022" sheetId="2" r:id="rId2"/>
+    <sheet name="MaddenCo Data 02-10-2022" sheetId="1" r:id="rId1"/>
+    <sheet name="MaddenCo Count 02-10-2022" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>

</xml_diff>

<commit_message>
UI Connected, branched for amount of change
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="MaddenCo Data 02-10-2022" sheetId="1" r:id="rId1"/>
-    <sheet name="MaddenCo Count 02-10-2022" sheetId="2" r:id="rId2"/>
+    <sheet name="MaddenCo Data 02-15-2022" sheetId="1" r:id="rId1"/>
+    <sheet name="MaddenCo Count 02-15-2022" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>

</xml_diff>

<commit_message>
Update Excel Formats using Json for format storage
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="MaddenCo Data 02-15-2022" sheetId="1" r:id="rId1"/>
-    <sheet name="MaddenCo Count 02-15-2022" sheetId="2" r:id="rId2"/>
+    <sheet name="MaddenCo Data 02-16-2022" sheetId="1" r:id="rId1"/>
+    <sheet name="MaddenCo Count 02-16-2022" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>

</xml_diff>

<commit_message>
both file parsing in UI
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -7,15 +7,18 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="MaddenCo Data 02-16-2022" sheetId="1" r:id="rId1"/>
-    <sheet name="MaddenCo Count 02-16-2022" sheetId="2" r:id="rId2"/>
+    <sheet name="MaddenCo Daily Data 02-17-2022" sheetId="1" r:id="rId1"/>
+    <sheet name="MaddenCo All Data 02-17-2022" sheetId="2" r:id="rId2"/>
+    <sheet name="MaddenCo Daily Count 02-17-2022" sheetId="3" r:id="rId3"/>
+    <sheet name="MaddenCo All Count 02-17-2022" sheetId="4" r:id="rId4"/>
+    <sheet name="MaddenCo Total Count 02-17-2022" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="122">
   <si>
     <t>Date Created</t>
   </si>
@@ -44,6 +47,9 @@
     <t>Time Last Changed</t>
   </si>
   <si>
+    <t>W</t>
+  </si>
+  <si>
     <t>C</t>
   </si>
   <si>
@@ -53,15 +59,18 @@
     <t>O</t>
   </si>
   <si>
-    <t>W</t>
-  </si>
-  <si>
     <t>H</t>
   </si>
   <si>
     <t>S</t>
   </si>
   <si>
+    <t>U002SUSIE</t>
+  </si>
+  <si>
+    <t>U002RHONDA</t>
+  </si>
+  <si>
     <t>U002MARK</t>
   </si>
   <si>
@@ -74,9 +83,6 @@
     <t>U002RYANW</t>
   </si>
   <si>
-    <t>U002SUSIE</t>
-  </si>
-  <si>
     <t>U002RYAN</t>
   </si>
   <si>
@@ -89,7 +95,13 @@
     <t>U002SUZANN</t>
   </si>
   <si>
-    <t>U002RHONDA</t>
+    <t>14:01:37</t>
+  </si>
+  <si>
+    <t>16:02:52</t>
+  </si>
+  <si>
+    <t>17:04:56</t>
   </si>
   <si>
     <t>13:26:45</t>
@@ -233,6 +245,126 @@
     <t>16:58:41</t>
   </si>
   <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>U002RICH</t>
+  </si>
+  <si>
+    <t>U002DANA</t>
+  </si>
+  <si>
+    <t>U002DAVID</t>
+  </si>
+  <si>
+    <t>17:07:48</t>
+  </si>
+  <si>
+    <t>09:25:44</t>
+  </si>
+  <si>
+    <t>09:44:40</t>
+  </si>
+  <si>
+    <t>13:18:09</t>
+  </si>
+  <si>
+    <t>15:14:23</t>
+  </si>
+  <si>
+    <t>12:25:37</t>
+  </si>
+  <si>
+    <t>16:22:23</t>
+  </si>
+  <si>
+    <t>08:40:09</t>
+  </si>
+  <si>
+    <t>11:04:57</t>
+  </si>
+  <si>
+    <t>11:42:08</t>
+  </si>
+  <si>
+    <t>12:02:46</t>
+  </si>
+  <si>
+    <t>12:11:44</t>
+  </si>
+  <si>
+    <t>12:23:44</t>
+  </si>
+  <si>
+    <t>12:36:01</t>
+  </si>
+  <si>
+    <t>16:47:50</t>
+  </si>
+  <si>
+    <t>16:47:57</t>
+  </si>
+  <si>
+    <t>12:50:49</t>
+  </si>
+  <si>
+    <t>13:32:39</t>
+  </si>
+  <si>
+    <t>08:44:24</t>
+  </si>
+  <si>
+    <t>08:53:58</t>
+  </si>
+  <si>
+    <t>10:05:14</t>
+  </si>
+  <si>
+    <t>14:37:27</t>
+  </si>
+  <si>
+    <t>08:37:45</t>
+  </si>
+  <si>
+    <t>08:40:42</t>
+  </si>
+  <si>
+    <t>08:56:28</t>
+  </si>
+  <si>
+    <t>09:29:45</t>
+  </si>
+  <si>
+    <t>16:24:01</t>
+  </si>
+  <si>
+    <t>16:36:09</t>
+  </si>
+  <si>
+    <t>16:55:53</t>
+  </si>
+  <si>
+    <t>08:28:25</t>
+  </si>
+  <si>
+    <t>09:39:06</t>
+  </si>
+  <si>
+    <t>13:27:55</t>
+  </si>
+  <si>
+    <t>13:50:24</t>
+  </si>
+  <si>
+    <t>15:59:48</t>
+  </si>
+  <si>
+    <t>16:25:01</t>
+  </si>
+  <si>
+    <t>16:28:39</t>
+  </si>
+  <si>
     <t>Total</t>
   </si>
   <si>
@@ -243,6 +375,15 @@
   </si>
   <si>
     <t>Emails</t>
+  </si>
+  <si>
+    <t>key_0</t>
+  </si>
+  <si>
+    <t>None_x</t>
+  </si>
+  <si>
+    <t>None_y</t>
   </si>
 </sst>
 </file>
@@ -667,7 +808,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -720,17 +861,14 @@
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
+      <c r="C2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>142</v>
+        <v>1</v>
       </c>
       <c r="F2" s="2">
-        <v>507374</v>
+        <v>507412</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>15</v>
@@ -749,23 +887,20 @@
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
+      <c r="C3" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="D3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>142</v>
+        <v>1</v>
       </c>
       <c r="F3" s="2">
-        <v>507427</v>
+        <v>507428</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>26</v>
@@ -778,23 +913,23 @@
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
+      <c r="C4" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="D4" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1">
         <v>142</v>
       </c>
       <c r="F4" s="2">
-        <v>507391</v>
+        <v>507431</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>27</v>
@@ -805,25 +940,25 @@
         <v>20220106</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="1">
         <v>142</v>
       </c>
       <c r="F5" s="2">
-        <v>507421</v>
+        <v>507374</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>28</v>
@@ -840,19 +975,19 @@
         <v>13</v>
       </c>
       <c r="D6" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="1">
         <v>142</v>
       </c>
       <c r="F6" s="2">
-        <v>507415</v>
+        <v>507427</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>29</v>
@@ -863,25 +998,25 @@
         <v>20220106</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="1">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="F7" s="2">
-        <v>507372</v>
+        <v>507391</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>30</v>
@@ -892,25 +1027,25 @@
         <v>20220106</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="1">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="F8" s="2">
-        <v>507386</v>
+        <v>507421</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>31</v>
@@ -921,25 +1056,25 @@
         <v>20220106</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="1">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="F9" s="2">
-        <v>507401</v>
+        <v>507415</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>32</v>
@@ -950,22 +1085,22 @@
         <v>20220106</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="1">
         <v>154</v>
       </c>
       <c r="F10" s="2">
-        <v>507403</v>
+        <v>507372</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>19</v>
@@ -979,22 +1114,22 @@
         <v>20220106</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="1">
         <v>154</v>
       </c>
       <c r="F11" s="2">
-        <v>507405</v>
+        <v>507386</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>19</v>
@@ -1008,22 +1143,22 @@
         <v>20220106</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" s="1">
         <v>154</v>
       </c>
       <c r="F12" s="2">
-        <v>507422</v>
+        <v>507401</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>19</v>
@@ -1037,7 +1172,7 @@
         <v>20220106</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>13</v>
@@ -1049,13 +1184,13 @@
         <v>154</v>
       </c>
       <c r="F13" s="2">
-        <v>507416</v>
+        <v>507403</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>36</v>
@@ -1066,25 +1201,25 @@
         <v>20220106</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="1">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F14" s="2">
-        <v>507389</v>
+        <v>507405</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>37</v>
@@ -1095,25 +1230,25 @@
         <v>20220106</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="1">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F15" s="2">
-        <v>507399</v>
+        <v>507422</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>38</v>
@@ -1124,7 +1259,7 @@
         <v>20220106</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
@@ -1133,16 +1268,16 @@
         <v>1</v>
       </c>
       <c r="E16" s="1">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F16" s="2">
-        <v>507369</v>
+        <v>507416</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>39</v>
@@ -1153,25 +1288,25 @@
         <v>20220106</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" s="1">
         <v>161</v>
       </c>
       <c r="F17" s="2">
-        <v>507395</v>
+        <v>507389</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>40</v>
@@ -1182,25 +1317,25 @@
         <v>20220106</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" s="1">
         <v>161</v>
       </c>
       <c r="F18" s="2">
-        <v>507414</v>
+        <v>507399</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>41</v>
@@ -1211,25 +1346,25 @@
         <v>20220106</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="1">
-        <v>124</v>
+        <v>161</v>
       </c>
       <c r="F19" s="2">
-        <v>507377</v>
+        <v>507369</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>42</v>
@@ -1240,25 +1375,25 @@
         <v>20220106</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="1">
-        <v>124</v>
+        <v>161</v>
       </c>
       <c r="F20" s="2">
-        <v>507383</v>
+        <v>507395</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>43</v>
@@ -1269,25 +1404,25 @@
         <v>20220106</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="1">
-        <v>124</v>
+        <v>161</v>
       </c>
       <c r="F21" s="2">
-        <v>507381</v>
+        <v>507414</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>44</v>
@@ -1298,7 +1433,7 @@
         <v>20220106</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>14</v>
@@ -1310,13 +1445,13 @@
         <v>124</v>
       </c>
       <c r="F22" s="2">
-        <v>507376</v>
+        <v>507377</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>45</v>
@@ -1327,7 +1462,7 @@
         <v>20220106</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>14</v>
@@ -1339,13 +1474,13 @@
         <v>124</v>
       </c>
       <c r="F23" s="2">
-        <v>507390</v>
+        <v>507383</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>46</v>
@@ -1356,7 +1491,7 @@
         <v>20220106</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>14</v>
@@ -1368,13 +1503,13 @@
         <v>124</v>
       </c>
       <c r="F24" s="2">
-        <v>507394</v>
+        <v>507381</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>47</v>
@@ -1385,7 +1520,7 @@
         <v>20220106</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>14</v>
@@ -1397,13 +1532,13 @@
         <v>124</v>
       </c>
       <c r="F25" s="2">
-        <v>507418</v>
+        <v>507376</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>48</v>
@@ -1414,7 +1549,7 @@
         <v>20220106</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>14</v>
@@ -1426,13 +1561,13 @@
         <v>124</v>
       </c>
       <c r="F26" s="2">
-        <v>507425</v>
+        <v>507390</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>49</v>
@@ -1443,7 +1578,7 @@
         <v>20220106</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>14</v>
@@ -1455,13 +1590,13 @@
         <v>124</v>
       </c>
       <c r="F27" s="2">
-        <v>507426</v>
+        <v>507394</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>50</v>
@@ -1472,7 +1607,7 @@
         <v>20220106</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>14</v>
@@ -1484,13 +1619,13 @@
         <v>124</v>
       </c>
       <c r="F28" s="2">
-        <v>507430</v>
+        <v>507418</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>51</v>
@@ -1501,7 +1636,7 @@
         <v>20220106</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>14</v>
@@ -1513,13 +1648,13 @@
         <v>124</v>
       </c>
       <c r="F29" s="2">
-        <v>507408</v>
+        <v>507425</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>52</v>
@@ -1530,25 +1665,25 @@
         <v>20220106</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D30" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30" s="1">
         <v>124</v>
       </c>
       <c r="F30" s="2">
-        <v>507402</v>
+        <v>507426</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>53</v>
@@ -1559,25 +1694,25 @@
         <v>20220106</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D31" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31" s="1">
         <v>124</v>
       </c>
       <c r="F31" s="2">
-        <v>507410</v>
+        <v>507430</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>54</v>
@@ -1588,25 +1723,25 @@
         <v>20220106</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D32" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32" s="1">
         <v>124</v>
       </c>
       <c r="F32" s="2">
-        <v>507413</v>
+        <v>507408</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>55</v>
@@ -1617,25 +1752,25 @@
         <v>20220106</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D33" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" s="1">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="F33" s="2">
-        <v>507379</v>
+        <v>507402</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>56</v>
@@ -1646,25 +1781,25 @@
         <v>20220106</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D34" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34" s="1">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="F34" s="2">
-        <v>507380</v>
+        <v>507410</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>57</v>
@@ -1675,25 +1810,25 @@
         <v>20220106</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D35" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35" s="1">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="F35" s="2">
-        <v>507384</v>
+        <v>507413</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>58</v>
@@ -1704,7 +1839,7 @@
         <v>20220106</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>14</v>
@@ -1716,13 +1851,13 @@
         <v>138</v>
       </c>
       <c r="F36" s="2">
-        <v>507388</v>
+        <v>507379</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>59</v>
@@ -1733,7 +1868,7 @@
         <v>20220106</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>14</v>
@@ -1745,13 +1880,13 @@
         <v>138</v>
       </c>
       <c r="F37" s="2">
-        <v>507396</v>
+        <v>507380</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>60</v>
@@ -1762,7 +1897,7 @@
         <v>20220106</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>14</v>
@@ -1774,13 +1909,13 @@
         <v>138</v>
       </c>
       <c r="F38" s="2">
-        <v>507398</v>
+        <v>507384</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>61</v>
@@ -1791,7 +1926,7 @@
         <v>20220106</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>14</v>
@@ -1803,13 +1938,13 @@
         <v>138</v>
       </c>
       <c r="F39" s="2">
-        <v>507371</v>
+        <v>507388</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>62</v>
@@ -1820,7 +1955,7 @@
         <v>20220106</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>14</v>
@@ -1832,13 +1967,13 @@
         <v>138</v>
       </c>
       <c r="F40" s="2">
-        <v>507419</v>
+        <v>507396</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>63</v>
@@ -1849,7 +1984,7 @@
         <v>20220106</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>14</v>
@@ -1861,13 +1996,13 @@
         <v>138</v>
       </c>
       <c r="F41" s="2">
-        <v>507424</v>
+        <v>507398</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>64</v>
@@ -1878,7 +2013,7 @@
         <v>20220106</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>14</v>
@@ -1890,13 +2025,13 @@
         <v>138</v>
       </c>
       <c r="F42" s="2">
-        <v>507429</v>
+        <v>507371</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>65</v>
@@ -1907,25 +2042,25 @@
         <v>20220106</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D43" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43" s="1">
         <v>138</v>
       </c>
       <c r="F43" s="2">
-        <v>507409</v>
+        <v>507419</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>66</v>
@@ -1936,25 +2071,25 @@
         <v>20220106</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D44" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E44" s="1">
         <v>138</v>
       </c>
       <c r="F44" s="2">
-        <v>507367</v>
+        <v>507424</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>67</v>
@@ -1965,25 +2100,25 @@
         <v>20220106</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D45" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E45" s="1">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="F45" s="2">
-        <v>507411</v>
+        <v>507429</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>68</v>
@@ -1994,7 +2129,7 @@
         <v>20220106</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>14</v>
@@ -2003,16 +2138,16 @@
         <v>1</v>
       </c>
       <c r="E46" s="1">
-        <v>169</v>
+        <v>138</v>
       </c>
       <c r="F46" s="2">
-        <v>507392</v>
+        <v>507409</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>69</v>
@@ -2023,7 +2158,7 @@
         <v>20220106</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>14</v>
@@ -2032,16 +2167,16 @@
         <v>1</v>
       </c>
       <c r="E47" s="1">
-        <v>169</v>
+        <v>138</v>
       </c>
       <c r="F47" s="2">
-        <v>507385</v>
+        <v>507367</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>70</v>
@@ -2052,7 +2187,7 @@
         <v>20220106</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>14</v>
@@ -2061,19 +2196,106 @@
         <v>1</v>
       </c>
       <c r="E48" s="1">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="F48" s="2">
-        <v>507400</v>
+        <v>507411</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E49" s="1">
+        <v>169</v>
+      </c>
+      <c r="F49" s="2">
+        <v>507392</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E50" s="1">
+        <v>169</v>
+      </c>
+      <c r="F50" s="2">
+        <v>507385</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E51" s="1">
+        <v>169</v>
+      </c>
+      <c r="F51" s="2">
+        <v>507400</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2083,7 +2305,2548 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I87"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>507412</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>507428</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>142</v>
+      </c>
+      <c r="F4" s="2">
+        <v>507431</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1">
+        <v>20211019</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>153</v>
+      </c>
+      <c r="F5" s="2">
+        <v>502945</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>142</v>
+      </c>
+      <c r="F6" s="2">
+        <v>507374</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>142</v>
+      </c>
+      <c r="F7" s="2">
+        <v>507427</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1">
+        <v>20220105</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>142</v>
+      </c>
+      <c r="F8" s="2">
+        <v>507282</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>142</v>
+      </c>
+      <c r="F9" s="2">
+        <v>507391</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>142</v>
+      </c>
+      <c r="F10" s="2">
+        <v>507421</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>142</v>
+      </c>
+      <c r="F11" s="2">
+        <v>507415</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>154</v>
+      </c>
+      <c r="F12" s="2">
+        <v>507372</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>154</v>
+      </c>
+      <c r="F13" s="2">
+        <v>507386</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>154</v>
+      </c>
+      <c r="F14" s="2">
+        <v>507401</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>154</v>
+      </c>
+      <c r="F15" s="2">
+        <v>507403</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>154</v>
+      </c>
+      <c r="F16" s="2">
+        <v>507405</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>154</v>
+      </c>
+      <c r="F17" s="2">
+        <v>507422</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>154</v>
+      </c>
+      <c r="F18" s="2">
+        <v>507416</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>161</v>
+      </c>
+      <c r="F19" s="2">
+        <v>507389</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>161</v>
+      </c>
+      <c r="F20" s="2">
+        <v>507399</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>161</v>
+      </c>
+      <c r="F21" s="2">
+        <v>507369</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>161</v>
+      </c>
+      <c r="F22" s="2">
+        <v>507395</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>161</v>
+      </c>
+      <c r="F23" s="2">
+        <v>507414</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
+        <v>124</v>
+      </c>
+      <c r="F24" s="2">
+        <v>507377</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="1">
+        <v>20220105</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <v>124</v>
+      </c>
+      <c r="F25" s="2">
+        <v>507332</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <v>124</v>
+      </c>
+      <c r="F26" s="2">
+        <v>507383</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <v>124</v>
+      </c>
+      <c r="F27" s="2">
+        <v>507381</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1">
+        <v>124</v>
+      </c>
+      <c r="F28" s="2">
+        <v>507376</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1">
+        <v>124</v>
+      </c>
+      <c r="F29" s="2">
+        <v>507390</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>124</v>
+      </c>
+      <c r="F30" s="2">
+        <v>507394</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="1">
+        <v>20220105</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <v>124</v>
+      </c>
+      <c r="F31" s="2">
+        <v>507303</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="1">
+        <v>20220105</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>124</v>
+      </c>
+      <c r="F32" s="2">
+        <v>507336</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>124</v>
+      </c>
+      <c r="F33" s="2">
+        <v>507418</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1">
+        <v>124</v>
+      </c>
+      <c r="F34" s="2">
+        <v>507425</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1">
+        <v>124</v>
+      </c>
+      <c r="F35" s="2">
+        <v>507426</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1">
+        <v>124</v>
+      </c>
+      <c r="F36" s="2">
+        <v>507430</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" s="1">
+        <v>124</v>
+      </c>
+      <c r="F37" s="2">
+        <v>507408</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="1">
+        <v>20220105</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E38" s="1">
+        <v>124</v>
+      </c>
+      <c r="F38" s="2">
+        <v>507311</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E39" s="1">
+        <v>124</v>
+      </c>
+      <c r="F39" s="2">
+        <v>507402</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E40" s="1">
+        <v>124</v>
+      </c>
+      <c r="F40" s="2">
+        <v>507410</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="1">
+        <v>20211029</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E41" s="1">
+        <v>124</v>
+      </c>
+      <c r="F41" s="2">
+        <v>503678</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E42" s="1">
+        <v>124</v>
+      </c>
+      <c r="F42" s="2">
+        <v>507413</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="1">
+        <v>20211019</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E43" s="1">
+        <v>138</v>
+      </c>
+      <c r="F43" s="2">
+        <v>502895</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E44" s="1">
+        <v>138</v>
+      </c>
+      <c r="F44" s="2">
+        <v>507379</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E45" s="1">
+        <v>138</v>
+      </c>
+      <c r="F45" s="2">
+        <v>507380</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E46" s="1">
+        <v>138</v>
+      </c>
+      <c r="F46" s="2">
+        <v>507384</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E47" s="1">
+        <v>138</v>
+      </c>
+      <c r="F47" s="2">
+        <v>507388</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="1">
+        <v>20211111</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1">
+        <v>138</v>
+      </c>
+      <c r="F48" s="2">
+        <v>504483</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="1">
+        <v>20220104</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E49" s="1">
+        <v>138</v>
+      </c>
+      <c r="F49" s="2">
+        <v>507209</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1">
+        <v>138</v>
+      </c>
+      <c r="F50" s="2">
+        <v>507396</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="1">
+        <v>20220104</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1">
+        <v>138</v>
+      </c>
+      <c r="F51" s="2">
+        <v>507216</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E52" s="1">
+        <v>138</v>
+      </c>
+      <c r="F52" s="2">
+        <v>507398</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="1">
+        <v>20220104</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1">
+        <v>138</v>
+      </c>
+      <c r="F53" s="2">
+        <v>507227</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="1">
+        <v>20220104</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1">
+        <v>138</v>
+      </c>
+      <c r="F54" s="2">
+        <v>507234</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="1">
+        <v>20220105</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1">
+        <v>138</v>
+      </c>
+      <c r="F55" s="2">
+        <v>507340</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E56" s="1">
+        <v>138</v>
+      </c>
+      <c r="F56" s="2">
+        <v>507371</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1">
+        <v>138</v>
+      </c>
+      <c r="F57" s="2">
+        <v>507419</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1">
+        <v>138</v>
+      </c>
+      <c r="F58" s="2">
+        <v>507424</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="1">
+        <v>138</v>
+      </c>
+      <c r="F59" s="2">
+        <v>507429</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" s="1">
+        <v>20211220</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="1">
+        <v>138</v>
+      </c>
+      <c r="F60" s="2">
+        <v>506458</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" s="1">
+        <v>20211213</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" s="1">
+        <v>138</v>
+      </c>
+      <c r="F61" s="2">
+        <v>506042</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="1">
+        <v>20220105</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E62" s="1">
+        <v>138</v>
+      </c>
+      <c r="F62" s="2">
+        <v>507308</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" s="1">
+        <v>20211215</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E63" s="1">
+        <v>138</v>
+      </c>
+      <c r="F63" s="2">
+        <v>506231</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D64" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E64" s="1">
+        <v>138</v>
+      </c>
+      <c r="F64" s="2">
+        <v>507409</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D65" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E65" s="1">
+        <v>138</v>
+      </c>
+      <c r="F65" s="2">
+        <v>507367</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" s="1">
+        <v>20211206</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E66" s="1">
+        <v>149</v>
+      </c>
+      <c r="F66" s="2">
+        <v>505707</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" s="1">
+        <v>20211219</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D67" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" s="1">
+        <v>149</v>
+      </c>
+      <c r="F67" s="2">
+        <v>506434</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" s="1">
+        <v>20220105</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D68" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E68" s="1">
+        <v>149</v>
+      </c>
+      <c r="F68" s="2">
+        <v>507361</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" s="1">
+        <v>20211217</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D69" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69" s="1">
+        <v>149</v>
+      </c>
+      <c r="F69" s="2">
+        <v>506390</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" s="1">
+        <v>20211101</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D70" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E70" s="1">
+        <v>149</v>
+      </c>
+      <c r="F70" s="2">
+        <v>503704</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" s="1">
+        <v>20211217</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D71" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E71" s="1">
+        <v>149</v>
+      </c>
+      <c r="F71" s="2">
+        <v>506355</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" s="1">
+        <v>20220103</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D72" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E72" s="1">
+        <v>149</v>
+      </c>
+      <c r="F72" s="2">
+        <v>507130</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" s="1">
+        <v>20220104</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D73" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E73" s="1">
+        <v>149</v>
+      </c>
+      <c r="F73" s="2">
+        <v>507211</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D74" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E74" s="1">
+        <v>149</v>
+      </c>
+      <c r="F74" s="2">
+        <v>507411</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" s="1">
+        <v>20211217</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D75" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E75" s="1">
+        <v>149</v>
+      </c>
+      <c r="F75" s="2">
+        <v>506396</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" s="1">
+        <v>20220105</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D76" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E76" s="1">
+        <v>149</v>
+      </c>
+      <c r="F76" s="2">
+        <v>507345</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" s="1">
+        <v>20211229</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D77" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E77" s="1">
+        <v>149</v>
+      </c>
+      <c r="F77" s="2">
+        <v>506905</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78" s="1">
+        <v>20220105</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D78" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E78" s="1">
+        <v>169</v>
+      </c>
+      <c r="F78" s="2">
+        <v>507317</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79" s="1">
+        <v>20220105</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D79" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E79" s="1">
+        <v>169</v>
+      </c>
+      <c r="F79" s="2">
+        <v>507348</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80" s="1">
+        <v>20220103</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D80" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E80" s="1">
+        <v>169</v>
+      </c>
+      <c r="F80" s="2">
+        <v>507156</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81" s="1">
+        <v>20220105</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D81" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E81" s="1">
+        <v>169</v>
+      </c>
+      <c r="F81" s="2">
+        <v>507268</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9">
+      <c r="A82" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D82" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E82" s="1">
+        <v>169</v>
+      </c>
+      <c r="F82" s="2">
+        <v>507392</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
+      <c r="A83" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D83" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E83" s="1">
+        <v>169</v>
+      </c>
+      <c r="F83" s="2">
+        <v>507385</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="A84" s="1">
+        <v>20220105</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D84" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E84" s="1">
+        <v>169</v>
+      </c>
+      <c r="F84" s="2">
+        <v>507341</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I84" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85" s="1">
+        <v>20220105</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D85" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E85" s="1">
+        <v>169</v>
+      </c>
+      <c r="F85" s="2">
+        <v>507344</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="A86" s="1">
+        <v>20220105</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D86" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E86" s="1">
+        <v>169</v>
+      </c>
+      <c r="F86" s="2">
+        <v>507326</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I86" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
+      <c r="A87" s="1">
+        <v>20220106</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D87" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E87" s="1">
+        <v>169</v>
+      </c>
+      <c r="F87" s="2">
+        <v>507400</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I87" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2097,60 +4860,236 @@
     <col min="6" max="6" width="25.7109375" style="6" customWidth="1"/>
     <col min="7" max="7" width="25.7109375" style="5" customWidth="1"/>
     <col min="8" max="8" width="25.7109375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="B1" s="7">
+    <row r="1" spans="1:9">
+      <c r="B1" s="7"/>
+      <c r="C1" s="8">
         <v>142</v>
       </c>
+      <c r="D1" s="7">
+        <v>154</v>
+      </c>
+      <c r="E1" s="8">
+        <v>161</v>
+      </c>
+      <c r="F1" s="7">
+        <v>124</v>
+      </c>
+      <c r="G1" s="8">
+        <v>138</v>
+      </c>
+      <c r="H1" s="7">
+        <v>149</v>
+      </c>
+      <c r="I1" s="8">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="6">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5">
+        <v>6</v>
+      </c>
+      <c r="D2" s="6">
+        <v>7</v>
+      </c>
+      <c r="E2" s="5">
+        <v>5</v>
+      </c>
+      <c r="F2" s="6">
+        <v>14</v>
+      </c>
+      <c r="G2" s="5">
+        <v>12</v>
+      </c>
+      <c r="H2" s="6">
+        <v>1</v>
+      </c>
+      <c r="I2" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="6">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5">
+        <v>3</v>
+      </c>
+      <c r="D3" s="6">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5">
+        <v>3</v>
+      </c>
+      <c r="F3" s="6">
+        <v>4</v>
+      </c>
+      <c r="G3" s="5">
+        <v>8</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>3</v>
+      </c>
+      <c r="D4" s="6">
+        <v>4</v>
+      </c>
+      <c r="E4" s="5">
+        <v>2</v>
+      </c>
+      <c r="F4" s="6">
+        <v>10</v>
+      </c>
+      <c r="G4" s="5">
+        <v>4</v>
+      </c>
+      <c r="H4" s="6">
+        <v>1</v>
+      </c>
+      <c r="I4" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="6">
+        <v>2</v>
+      </c>
+      <c r="C5" s="5">
+        <v>3</v>
+      </c>
+      <c r="D5" s="6">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5">
+        <v>3</v>
+      </c>
+      <c r="F5" s="6">
+        <v>3</v>
+      </c>
+      <c r="G5" s="5">
+        <v>2</v>
+      </c>
+      <c r="H5" s="6">
+        <v>1</v>
+      </c>
+      <c r="I5" s="5">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="25.7109375" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="B1" s="7"/>
       <c r="C1" s="8">
+        <v>142</v>
+      </c>
+      <c r="D1" s="7">
+        <v>153</v>
+      </c>
+      <c r="E1" s="8">
         <v>154</v>
       </c>
-      <c r="D1" s="7">
+      <c r="F1" s="7">
         <v>161</v>
       </c>
-      <c r="E1" s="8">
+      <c r="G1" s="8">
         <v>124</v>
       </c>
-      <c r="F1" s="7">
+      <c r="H1" s="7">
         <v>138</v>
       </c>
-      <c r="G1" s="8">
+      <c r="I1" s="8">
         <v>149</v>
       </c>
-      <c r="H1" s="7">
+      <c r="J1" s="7">
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:10">
       <c r="A2" s="8" t="s">
-        <v>72</v>
+        <v>115</v>
       </c>
       <c r="B2" s="6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2" s="5">
         <v>7</v>
       </c>
       <c r="D2" s="6">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5">
+        <v>7</v>
+      </c>
+      <c r="F2" s="6">
         <v>5</v>
       </c>
-      <c r="E2" s="5">
-        <v>14</v>
-      </c>
-      <c r="F2" s="6">
+      <c r="G2" s="5">
+        <v>19</v>
+      </c>
+      <c r="H2" s="6">
+        <v>23</v>
+      </c>
+      <c r="I2" s="5">
         <v>12</v>
       </c>
-      <c r="G2" s="5">
-        <v>1</v>
-      </c>
-      <c r="H2" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="J2" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="8" t="s">
-        <v>73</v>
+        <v>116</v>
       </c>
       <c r="B3" s="6">
         <v>2</v>
@@ -2159,71 +5098,151 @@
         <v>3</v>
       </c>
       <c r="D3" s="6">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
         <v>3</v>
       </c>
-      <c r="E3" s="5">
-        <v>4</v>
-      </c>
       <c r="F3" s="6">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G3" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H3" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>11</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="8" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="B4" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C4" s="5">
         <v>4</v>
       </c>
       <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5">
+        <v>4</v>
+      </c>
+      <c r="F4" s="6">
         <v>2</v>
       </c>
-      <c r="E4" s="5">
-        <v>10</v>
-      </c>
-      <c r="F4" s="6">
-        <v>4</v>
-      </c>
       <c r="G4" s="5">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="H4" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>12</v>
+      </c>
+      <c r="I4" s="5">
+        <v>12</v>
+      </c>
+      <c r="J4" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="8" t="s">
-        <v>75</v>
+        <v>118</v>
       </c>
       <c r="B5" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="5">
         <v>4</v>
       </c>
       <c r="D5" s="6">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="6">
         <v>3</v>
       </c>
-      <c r="E5" s="5">
-        <v>3</v>
-      </c>
-      <c r="F5" s="6">
-        <v>2</v>
-      </c>
       <c r="G5" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H5" s="6">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="I5" s="5">
+        <v>8</v>
+      </c>
+      <c r="J5" s="6">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="25.7109375" style="6" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" style="5" customWidth="1"/>
+    <col min="12" max="12" width="25.7109375" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12">
+      <c r="B1" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" s="7">
+        <v>142</v>
+      </c>
+      <c r="E1" s="8">
+        <v>153</v>
+      </c>
+      <c r="F1" s="7">
+        <v>154</v>
+      </c>
+      <c r="G1" s="8">
+        <v>161</v>
+      </c>
+      <c r="H1" s="7">
+        <v>124</v>
+      </c>
+      <c r="I1" s="8">
+        <v>138</v>
+      </c>
+      <c r="J1" s="7">
+        <v>149</v>
+      </c>
+      <c r="K1" s="8">
+        <v>169</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>